<commit_message>
3 fake registered people
</commit_message>
<xml_diff>
--- a/Harrys Portfolio/houses for advertising.xlsx
+++ b/Harrys Portfolio/houses for advertising.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>houseid</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Stafford Heights</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>9 Hetherington</t>
+  </si>
+  <si>
+    <t>Herston</t>
   </si>
 </sst>
 </file>
@@ -496,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,6 +869,41 @@
         <v>380</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>432594785</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11">
+        <v>4006</v>
+      </c>
+      <c r="K11">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>